<commit_message>
config database and static, templates folder for flask call this from frontend
</commit_message>
<xml_diff>
--- a/backend/uploads/test_docs/Book2.xlsx
+++ b/backend/uploads/test_docs/Book2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aob\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\2020\sem2_62\SE2\SE-Project\Project\backend\uploads\test_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{16B84744-F56E-4EEC-BE6E-DDBB362C690F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A65DBC-6EC4-4E05-A4CB-EF8C77D888C5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{58DA6C14-4C95-45DF-9C69-707B26BF0E0D}"/>
   </bookViews>
@@ -33,10 +33,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>aaa</t>
+    <t>name</t>
   </si>
   <si>
-    <t>dddd</t>
+    <t>author</t>
   </si>
 </sst>
 </file>
@@ -391,7 +391,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,7 +409,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -417,7 +417,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -425,7 +425,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -433,7 +433,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -441,7 +441,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>